<commit_message>
Added my contributions to GL project tracker
</commit_message>
<xml_diff>
--- a/Game Logic Team/Project tracker (GL Team).xlsx
+++ b/Game Logic Team/Project tracker (GL Team).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD4EABD-B080-4634-B65B-3FF6BE728D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{905EDE77-CEFB-45C6-A9D2-08634384932B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="12777" windowHeight="13536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project tracker" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Category</t>
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Category 1</t>
   </si>
   <si>
     <t>Category 2</t>
@@ -118,15 +115,9 @@
     <t>Project Task Tracker</t>
   </si>
   <si>
-    <t>Student 1</t>
-  </si>
-  <si>
     <t>Student 2</t>
   </si>
   <si>
-    <t>Student 3</t>
-  </si>
-  <si>
     <t>Student 5</t>
   </si>
   <si>
@@ -206,6 +197,33 @@
   </si>
   <si>
     <t>30-10-2031</t>
+  </si>
+  <si>
+    <t>Alyvia</t>
+  </si>
+  <si>
+    <t>Holden</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Ezra</t>
+  </si>
+  <si>
+    <t>01-11-2024</t>
+  </si>
+  <si>
+    <t>31-10-2024</t>
+  </si>
+  <si>
+    <t>9:00-11:30pm on nov 1st</t>
+  </si>
+  <si>
+    <t>7:00-9:00pm on nov 1st</t>
+  </si>
+  <si>
+    <t>5:00-7:00pm on oct 30th, 6:00-7:00 on nov 1st</t>
   </si>
 </sst>
 </file>
@@ -556,7 +574,7 @@
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -640,6 +658,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1555,25 +1576,25 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="29.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" style="3" customWidth="1"/>
-    <col min="2" max="4" width="18.69921875" style="19" customWidth="1"/>
-    <col min="5" max="6" width="18.69921875" style="20" customWidth="1"/>
-    <col min="7" max="8" width="18.69921875" style="19" customWidth="1"/>
-    <col min="9" max="10" width="16.796875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="18.7265625" style="19" customWidth="1"/>
+    <col min="5" max="6" width="18.7265625" style="20" customWidth="1"/>
+    <col min="7" max="8" width="18.7265625" style="19" customWidth="1"/>
+    <col min="9" max="10" width="16.81640625" style="20" customWidth="1"/>
     <col min="11" max="12" width="16" style="19" customWidth="1"/>
-    <col min="13" max="13" width="20.3984375" style="19" customWidth="1"/>
-    <col min="14" max="14" width="6.69921875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="4.19921875" style="2" customWidth="1"/>
-    <col min="16" max="40" width="3.296875" style="2" customWidth="1"/>
-    <col min="41" max="16384" width="9.09765625" style="2"/>
+    <col min="13" max="13" width="20.36328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="4.1796875" style="2" customWidth="1"/>
+    <col min="16" max="40" width="3.26953125" style="2" customWidth="1"/>
+    <col min="41" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1589,16 +1610,16 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="80.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="9">
         <v>0.25</v>
@@ -1611,7 +1632,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1627,62 +1648,62 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="62.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="24" t="s">
+      <c r="H4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="17" t="s">
         <v>15</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>16</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" s="18">
         <v>6</v>
@@ -1690,32 +1711,39 @@
       <c r="H5" s="21">
         <v>3</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="21" t="str">
-        <f>IF(COUNTA('Project tracker'!$I5,'Project tracker'!$J5)&lt;&gt;2,"",DAYS360('Project tracker'!$I5,'Project tracker'!$J5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="M5" s="18"/>
+      <c r="I5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="28">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G6" s="18">
         <v>6</v>
@@ -1723,32 +1751,39 @@
       <c r="H6" s="21">
         <v>3</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="21" t="str">
-        <f>IF(COUNTA('Project tracker'!$I6,'Project tracker'!$J6)&lt;&gt;2,"",DAYS360('Project tracker'!$I6,'Project tracker'!$J6,FALSE))</f>
-        <v/>
-      </c>
-      <c r="M6" s="18"/>
+      <c r="I6" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="28">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L6" s="21">
+        <v>2</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G7" s="18">
         <v>6</v>
@@ -1756,32 +1791,39 @@
       <c r="H7" s="21">
         <v>3</v>
       </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="21" t="str">
-        <f>IF(COUNTA('Project tracker'!$I7,'Project tracker'!$J7)&lt;&gt;2,"",DAYS360('Project tracker'!$I7,'Project tracker'!$J7,FALSE))</f>
-        <v/>
-      </c>
-      <c r="M7" s="18"/>
+      <c r="I7" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="L7" s="21">
+        <v>2</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G8" s="18">
         <v>6</v>
@@ -1799,22 +1841,22 @@
       <c r="M8" s="18"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" s="18">
         <v>6</v>
@@ -1832,22 +1874,22 @@
       <c r="M9" s="18"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G10" s="18">
         <v>6</v>
@@ -1865,22 +1907,22 @@
       <c r="M10" s="18"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>47</v>
       </c>
       <c r="G11" s="18">
         <v>6</v>
@@ -1898,22 +1940,22 @@
       <c r="M11" s="18"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G12" s="18">
         <v>6</v>
@@ -1931,22 +1973,22 @@
       <c r="M12" s="18"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G13" s="18">
         <v>6</v>
@@ -1964,7 +2006,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -2032,38 +2074,38 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="20.09765625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="16.69921875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.69921875" style="27"/>
+    <col min="1" max="1" width="12.7265625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2081,108 +2123,108 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="29.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" style="12" customWidth="1"/>
-    <col min="2" max="3" width="18.5" style="23" customWidth="1"/>
-    <col min="4" max="4" width="6.69921875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" style="12" customWidth="1"/>
+    <col min="2" max="3" width="18.453125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="13" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" customFormat="1" ht="80.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:4" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" customFormat="1" ht="62.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" customFormat="1" ht="33.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" customFormat="1" ht="29.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -2204,6 +2246,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2221,15 +2272,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2545,6 +2587,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9066C173-72E5-4455-ACFB-9A7596D30A2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2552,14 +2602,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>